<commit_message>
third class on faeture engineering
</commit_message>
<xml_diff>
--- a/assignments/module_2/task_2/craves_dataset.xlsx
+++ b/assignments/module_2/task_2/craves_dataset.xlsx
@@ -30,9 +30,6 @@
     <t>Flavor</t>
   </si>
   <si>
-    <t>Paxkage size</t>
-  </si>
-  <si>
     <t>Weight (g)</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Available</t>
+  </si>
+  <si>
+    <t>Package size</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,16 +461,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -478,16 +478,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
       </c>
       <c r="F2">
         <v>250</v>
@@ -496,7 +496,7 @@
         <v>2500</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -504,16 +504,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
       <c r="F3">
         <v>300</v>
@@ -522,7 +522,7 @@
         <v>3000</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -530,16 +530,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>300</v>
@@ -548,7 +548,7 @@
         <v>4000</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -556,16 +556,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5">
         <v>600</v>
@@ -574,7 +574,7 @@
         <v>4500</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -582,16 +582,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>300</v>
@@ -600,7 +600,7 @@
         <v>2500</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>